<commit_message>
復 and other comps
added a few components to categorize 5 kanji as VR
</commit_message>
<xml_diff>
--- a/freq/1,200 KANJI.xlsx
+++ b/freq/1,200 KANJI.xlsx
@@ -8,15 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kandr\Projects\kanji-mbo\freq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E105C6AD-9A9A-4854-997B-A0897CD0AFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB104BFF-2283-4222-BEE8-9DC00B478AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5193" uniqueCount="3572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5197" uniqueCount="3574">
   <si>
     <t>Kanji</t>
   </si>
@@ -11064,6 +11075,36 @@
         <family val="2"/>
       </rPr>
       <t>ジョウ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ハン、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>バン</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ケン、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ゲン</t>
     </r>
   </si>
 </sst>
@@ -11679,7 +11720,7 @@
   <dimension ref="A1:H1205"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A628" sqref="A628"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="24" zeroHeight="1" x14ac:dyDescent="0.5"/>
@@ -11990,7 +12031,7 @@
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="10" t="s">
-        <v>61</v>
+        <v>3573</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>62</v>
@@ -19712,9 +19753,11 @@
         <v>195</v>
       </c>
       <c r="C395" s="14" t="s">
-        <v>1363</v>
-      </c>
-      <c r="D395" s="11"/>
+        <v>973</v>
+      </c>
+      <c r="D395" s="11" t="s">
+        <v>597</v>
+      </c>
       <c r="E395" s="10" t="s">
         <v>974</v>
       </c>
@@ -20872,9 +20915,11 @@
         <v>117</v>
       </c>
       <c r="C451" s="14" t="s">
-        <v>1534</v>
-      </c>
-      <c r="D451" s="11"/>
+        <v>979</v>
+      </c>
+      <c r="D451" s="11" t="s">
+        <v>1106</v>
+      </c>
       <c r="E451" s="10" t="s">
         <v>507</v>
       </c>
@@ -23012,8 +23057,12 @@
       <c r="A556" s="10" t="s">
         <v>1838</v>
       </c>
-      <c r="B556" s="11"/>
-      <c r="C556" s="11"/>
+      <c r="B556" s="11" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C556" s="11" t="s">
+        <v>2610</v>
+      </c>
       <c r="D556" s="11"/>
       <c r="E556" s="10" t="s">
         <v>1412</v>
@@ -26368,7 +26417,7 @@
       <c r="C716" s="11"/>
       <c r="D716" s="11"/>
       <c r="E716" s="10" t="s">
-        <v>865</v>
+        <v>3572</v>
       </c>
       <c r="F716" s="12"/>
       <c r="G716" s="13" t="s">
@@ -36485,7 +36534,7 @@
         <v>3566</v>
       </c>
       <c r="H1201" s="5">
-        <v>1752.6</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="1202" spans="1:8" x14ac:dyDescent="0.5"/>

</xml_diff>